<commit_message>
updated the read do file to create new variables and updated the mock tables
</commit_message>
<xml_diff>
--- a/tables/mockup_tables.xlsx
+++ b/tables/mockup_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissoria/Documents/Research/us_international_ses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F5ADEE-6315-3A45-8F4E-C5C1044CB1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972FA714-DD9D-1946-9514-3245CE1BDD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41360" yWindow="-4100" windowWidth="35320" windowHeight="17440" xr2:uid="{9D8D573E-D8BA-534D-B99F-F55EF3DAE25F}"/>
+    <workbookView xWindow="40720" yWindow="-3900" windowWidth="35320" windowHeight="17440" activeTab="2" xr2:uid="{9D8D573E-D8BA-534D-B99F-F55EF3DAE25F}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
   <si>
     <t>Cuba</t>
   </si>
@@ -152,13 +152,19 @@
   </si>
   <si>
     <t>Foreign Hispanic</t>
+  </si>
+  <si>
+    <t>Ages 60-69</t>
+  </si>
+  <si>
+    <t>Ages 70-79</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,12 +178,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,13 +273,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -288,7 +287,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -640,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA773FD-D638-C948-9DD6-92F46F5314E3}">
   <dimension ref="A2:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="A3:J26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,34 +658,34 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
@@ -711,16 +709,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="A7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
@@ -746,26 +735,26 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -781,8 +770,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
@@ -808,26 +797,26 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
@@ -844,15 +833,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
@@ -885,28 +866,28 @@
     <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -930,18 +911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>12</v>
       </c>
@@ -949,13 +919,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="3" t="s">
         <v>9</v>
@@ -971,13 +941,14 @@
   <dimension ref="A2:L69"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
@@ -992,31 +963,31 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1030,7 +1001,6 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
@@ -1038,7 +1008,6 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
@@ -1046,20 +1015,9 @@
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="A7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
@@ -1069,7 +1027,6 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
@@ -1077,7 +1034,6 @@
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -1085,30 +1041,29 @@
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1116,7 +1071,6 @@
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -1124,10 +1078,9 @@
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
@@ -1137,7 +1090,6 @@
       <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
@@ -1145,7 +1097,6 @@
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -1153,30 +1104,29 @@
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
@@ -1184,7 +1134,6 @@
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -1192,19 +1141,9 @@
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
@@ -1214,7 +1153,6 @@
       <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
@@ -1222,7 +1160,6 @@
       <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
@@ -1230,7 +1167,6 @@
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1240,31 +1176,31 @@
     <row r="29" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1288,19 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>12</v>
       </c>
@@ -1308,268 +1232,225 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="1"/>
+      <c r="D39" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="F39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="G39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="H39" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="C40" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="9"/>
+      <c r="C44" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="C48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="2"/>
+      <c r="C50" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="9"/>
+      <c r="C52" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="5"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+      <c r="C53" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="C56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="9"/>
+      <c r="C60" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="2"/>
+      <c r="C62" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="9"/>
+      <c r="C64" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="5"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C68" s="9"/>
+      <c r="C68" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="5"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="2"/>
+      <c r="C69" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1581,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A7B5D8-4364-9F4C-A02E-4108C882E048}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,22 +1480,22 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1638,16 +1519,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>12</v>
@@ -1671,10 +1542,10 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1697,12 +1568,6 @@
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">

</xml_diff>